<commit_message>
Done, u can check and change
</commit_message>
<xml_diff>
--- a/assignments/hw4/answers/results/charts.xlsx
+++ b/assignments/hw4/answers/results/charts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louki\Desktop\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucy-my.sharepoint.com/personal/cseas002_ucy_ac_cy/Documents/UCY/EPL_499-Datacenters/cs499-fa22/assignments/hw4/answers/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A7070A-73E2-4086-819C-D668E6E1CE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{52A7070A-73E2-4086-819C-D668E6E1CE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50B6E651-10CF-47DA-BF44-49E222B39590}"/>
   <bookViews>
-    <workbookView xWindow="33555" yWindow="2595" windowWidth="17250" windowHeight="8865" xr2:uid="{A75B0D03-1F87-4EDB-9D08-6843AC327B5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="487" xr2:uid="{A75B0D03-1F87-4EDB-9D08-6843AC327B5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Single</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Latency</t>
+  </si>
+  <si>
+    <t>Not Scaled</t>
+  </si>
+  <si>
+    <t>Scaled</t>
   </si>
 </sst>
 </file>
@@ -102,10 +108,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,7 +335,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -936,6 +942,721 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Latency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Latency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$2:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Not Scaled</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Scaled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.9347999999999983</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8208000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-806C-42F7-8C46-B786C035FF50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="563977312"/>
+        <c:axId val="563973984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="563977312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563973984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="563973984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Milliseconds (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563977312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Throughput</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Throughput</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$2:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Not Scaled</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Scaled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D760-4971-BA11-704F42C170A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="605362768"/>
+        <c:axId val="605352784"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="605362768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="605352784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="605352784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Requests</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> per Second </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="605362768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1016,6 +1737,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1695,6 +2496,1012 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2117,6 +3924,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE8C8CC-8E07-A219-6D1F-CB83C2BD0DD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>461962</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CDF6FD7-64E9-160D-F640-2C8DC5DC9E14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2422,20 +4301,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B883049-5561-4DBD-AFBE-7547AF4B121D}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -2445,8 +4326,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2456,8 +4343,17 @@
       <c r="C2">
         <v>331.32</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>5.9347999999999983</v>
+      </c>
+      <c r="K2">
+        <v>1030</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2467,8 +4363,56 @@
       <c r="C3">
         <v>412.18</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>4.8208000000000002</v>
+      </c>
+      <c r="K3">
+        <v>1030</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -2478,8 +4422,9 @@
       <c r="C22" t="s">
         <v>1</v>
       </c>
+      <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2489,8 +4434,9 @@
       <c r="C23">
         <v>0.98</v>
       </c>
+      <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -2500,9 +4446,83 @@
       <c r="C24">
         <v>0.97</v>
       </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>